<commit_message>
Se agregan referencias en el archivo
</commit_message>
<xml_diff>
--- a/SIMULADORES EXCEL/TMR1 CALCULADOR DE TIEMPO.xlsx
+++ b/SIMULADORES EXCEL/TMR1 CALCULADOR DE TIEMPO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lujeo\Documents\Atmel Studio\7.0\GccApplication1\EjemploAvr\SIMULADORES EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{697C6BD3-973F-42EB-82A9-BF1333FC09C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B9CF28-0619-4AD9-8256-AF7AE4076BC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7A04CE77-AAA7-482E-897D-0CB6AC153F1B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Fclock</t>
   </si>
@@ -50,15 +50,31 @@
   <si>
     <t>T RETARDO</t>
   </si>
+  <si>
+    <t>Referencias</t>
+  </si>
+  <si>
+    <t>pag 99</t>
+  </si>
+  <si>
+    <t>datasheet atmega32</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,12 +127,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,8 +161,8 @@
       <xdr:rowOff>65563</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4292633" cy="614784"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -284,7 +301,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -655,15 +672,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08AFBDA-9152-4F21-BD05-436E7DC06C49}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -671,7 +688,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -680,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -689,7 +706,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -697,7 +714,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -706,8 +723,20 @@
         <v>31249</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
El programa ejecuta un contador del 0 al 99
</commit_message>
<xml_diff>
--- a/SIMULADORES EXCEL/TMR1 CALCULADOR DE TIEMPO.xlsx
+++ b/SIMULADORES EXCEL/TMR1 CALCULADOR DE TIEMPO.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lujeo\Documents\Atmel Studio\7.0\GccApplication1\EjemploAvr\SIMULADORES EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B9CF28-0619-4AD9-8256-AF7AE4076BC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2865C0EB-E613-4A2E-927C-C80E42376567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7A04CE77-AAA7-482E-897D-0CB6AC153F1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7A04CE77-AAA7-482E-897D-0CB6AC153F1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
+    <sheet name="bcd_2_7seg" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Fclock</t>
   </si>
@@ -58,6 +60,36 @@
   </si>
   <si>
     <t>datasheet atmega32</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>dot</t>
+  </si>
+  <si>
+    <t>Binario</t>
+  </si>
+  <si>
+    <t>admux register</t>
   </si>
 </sst>
 </file>
@@ -80,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,8 +131,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -123,22 +161,195 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -672,32 +883,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08AFBDA-9152-4F21-BD05-436E7DC06C49}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4">
         <f>1/B1</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -706,7 +917,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -714,16 +925,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1">
         <f>B3/(2*B4*B2)-1</f>
-        <v>31249</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6249</v>
+      </c>
+      <c r="D6">
+        <f>POWER(2,16)</f>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
@@ -739,4 +954,176 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F037A6E0-1701-4A68-98EC-8D7AE9EE2A1D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F1F917-328A-44CD-A968-88B7C1908FC8}">
+  <dimension ref="B1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="3.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4" customWidth="1"/>
+    <col min="5" max="5" width="1.28515625" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" customWidth="1"/>
+    <col min="7" max="14" width="6.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11"/>
+    </row>
+    <row r="3" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="2:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14"/>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="2:15" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="15"/>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="18"/>
+    </row>
+    <row r="7" spans="2:15" ht="36.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f>F6</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>C4</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>B3</f>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f>B5</f>
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>C6</f>
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <f>D5</f>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f>D3</f>
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <f>C2</f>
+        <v>1</v>
+      </c>
+      <c r="O9" t="str">
+        <f>_xlfn.CONCAT("0b"&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9)</f>
+        <v>0b00111111</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2 D3 D5 C6 B5 C4 B3 F6">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se termina el Programa con el ADC
</commit_message>
<xml_diff>
--- a/SIMULADORES EXCEL/TMR1 CALCULADOR DE TIEMPO.xlsx
+++ b/SIMULADORES EXCEL/TMR1 CALCULADOR DE TIEMPO.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lujeo\Documents\Atmel Studio\7.0\GccApplication1\EjemploAvr\SIMULADORES EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2865C0EB-E613-4A2E-927C-C80E42376567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9DCF58-FAC4-48E2-8ACE-B7127F00CC4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{7A04CE77-AAA7-482E-897D-0CB6AC153F1B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{7A04CE77-AAA7-482E-897D-0CB6AC153F1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
-    <sheet name="bcd_2_7seg" sheetId="2" r:id="rId3"/>
+    <sheet name="bcd_2_7seg" sheetId="2" r:id="rId2"/>
+    <sheet name="Referencias del adc" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Fclock</t>
   </si>
@@ -90,6 +90,33 @@
   </si>
   <si>
     <t>admux register</t>
+  </si>
+  <si>
+    <t>ADCH</t>
+  </si>
+  <si>
+    <t>ADCL</t>
+  </si>
+  <si>
+    <t>ADSC REGISTER</t>
+  </si>
+  <si>
+    <t>ADCSRA</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>SREG</t>
+  </si>
+  <si>
+    <t>fclk</t>
+  </si>
+  <si>
+    <t>Prescales</t>
+  </si>
+  <si>
+    <t>fadc</t>
   </si>
 </sst>
 </file>
@@ -318,17 +345,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -957,26 +974,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F037A6E0-1701-4A68-98EC-8D7AE9EE2A1D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F1F917-328A-44CD-A968-88B7C1908FC8}">
   <dimension ref="B1:O9"/>
   <sheetViews>
@@ -1116,14 +1113,158 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2 D3 D5 C6 B5 C4 B3 F6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F037A6E0-1701-4A68-98EC-8D7AE9EE2A1D}">
+  <dimension ref="A1:U19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="16" width="5.140625" customWidth="1"/>
+    <col min="17" max="22" width="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>1</v>
+      </c>
+      <c r="R3" s="2">
+        <v>1</v>
+      </c>
+      <c r="S3" s="2">
+        <v>1</v>
+      </c>
+      <c r="T3" s="2">
+        <v>1</v>
+      </c>
+      <c r="U3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1000000</v>
+      </c>
+      <c r="D8">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>C8/D8</f>
+        <v>7812.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>1023</v>
+      </c>
+      <c r="D16">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <f>C16/D16</f>
+        <v>10.333333333333334</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>1023</v>
+      </c>
+      <c r="D19">
+        <f>C19/D18</f>
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>